<commit_message>
db validation added for delete User and UserSkillMap API
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/user_testdata.xlsx
+++ b/src/test/resources/excel/user_testdata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diana\git\BDDRestAssuredUserAPITeamBJan22\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diana\git\NinjaCoderLMSRestAssured\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF6AC38-7E8D-49F9-892C-233A25E4F15F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DE0518-E32D-4621-B845-612C1A96E178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="put" sheetId="2" r:id="rId3"/>
     <sheet name="delete" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -466,7 +466,7 @@
     <t>201</t>
   </si>
   <si>
-    <t>U297</t>
+    <t>U145</t>
   </si>
 </sst>
 </file>
@@ -1404,7 +1404,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>